<commit_message>
Change C211, C212 from 0402 to 0805
</commit_message>
<xml_diff>
--- a/hardware/edm_control_board/documents/edm_control_board_bom.xlsx
+++ b/hardware/edm_control_board/documents/edm_control_board_bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23340" windowHeight="13260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23340" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="edm_control_board._1" localSheetId="0">Sheet1!$B$1:$F$28</definedName>
+    <definedName name="edm_control_board._1" localSheetId="0">Sheet1!$A$1:$E$28</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,8 +27,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="edm_control_board" type="6" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="edm_control_board" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\development\github\EDM\hardware\edm_control_board\cad\edm_control_board." decimal="," thousands=" " tab="0" comma="1">
       <textFields count="2">
         <textField/>
@@ -213,9 +213,6 @@
     <t>C212, C211</t>
   </si>
   <si>
-    <t>311-1442-1-ND</t>
-  </si>
-  <si>
     <t>C301, C302</t>
   </si>
   <si>
@@ -358,12 +355,15 @@
   </si>
   <si>
     <t>497-17184-ND</t>
+  </si>
+  <si>
+    <t>311-3425-1-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -413,7 +413,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="edm_control_board._1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="edm_control_board._1" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -712,455 +712,460 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" activeCellId="1" sqref="D6 D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" customWidth="1"/>
-    <col min="6" max="6" width="62" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" customWidth="1"/>
+    <col min="5" max="5" width="62" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2">
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12">
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21">
         <v>4</v>
       </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C14">
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22">
         <v>4</v>
       </c>
-      <c r="D14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" t="s">
-        <v>77</v>
-      </c>
-      <c r="F15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16">
-        <v>6</v>
-      </c>
-      <c r="D16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>84</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" t="s">
-        <v>85</v>
-      </c>
-      <c r="F19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" t="s">
-        <v>87</v>
-      </c>
-      <c r="F20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
         <v>103</v>
       </c>
-      <c r="F21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>89</v>
       </c>
-      <c r="C22">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" t="s">
         <v>104</v>
       </c>
-      <c r="F22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="E23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>90</v>
       </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" t="s">
-        <v>105</v>
-      </c>
-      <c r="F23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s">
         <v>91</v>
       </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>41</v>
-      </c>
       <c r="E24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>92</v>
       </c>
-      <c r="F24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" t="s">
         <v>93</v>
       </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>43</v>
-      </c>
       <c r="E25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>94</v>
       </c>
-      <c r="F25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
         <v>95</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
       </c>
       <c r="D26" t="s">
         <v>96</v>
@@ -1168,46 +1173,43 @@
       <c r="E26" t="s">
         <v>97</v>
       </c>
-      <c r="F26" t="s">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" t="s">
         <v>99</v>
       </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>45</v>
-      </c>
       <c r="E27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>100</v>
       </c>
-      <c r="F27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" t="s">
         <v>101</v>
       </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
-        <v>47</v>
-      </c>
       <c r="E28" t="s">
-        <v>102</v>
-      </c>
-      <c r="F28" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="72" orientation="landscape" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change C208, C210 from 0402 to 0805
</commit_message>
<xml_diff>
--- a/hardware/edm_control_board/documents/edm_control_board_bom.xlsx
+++ b/hardware/edm_control_board/documents/edm_control_board_bom.xlsx
@@ -207,9 +207,6 @@
     <t>C210, C208</t>
   </si>
   <si>
-    <t>311-1641-1-ND</t>
-  </si>
-  <si>
     <t>C212, C211</t>
   </si>
   <si>
@@ -358,6 +355,9 @@
   </si>
   <si>
     <t>311-3425-1-ND</t>
+  </si>
+  <si>
+    <t>311-1100-1-ND</t>
   </si>
 </sst>
 </file>
@@ -719,7 +719,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" activeCellId="1" sqref="D6 D5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,7 +794,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -802,7 +802,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -811,7 +811,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -819,7 +819,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -828,7 +828,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
@@ -836,7 +836,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -845,7 +845,7 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
@@ -853,7 +853,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -862,7 +862,7 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -879,7 +879,7 @@
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -896,7 +896,7 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
         <v>16</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -913,7 +913,7 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
         <v>18</v>
@@ -921,7 +921,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -930,7 +930,7 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E12" t="s">
         <v>20</v>
@@ -938,7 +938,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -947,7 +947,7 @@
         <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
         <v>22</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -964,7 +964,7 @@
         <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
         <v>24</v>
@@ -972,7 +972,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -981,7 +981,7 @@
         <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E15" t="s">
         <v>26</v>
@@ -989,7 +989,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -998,7 +998,7 @@
         <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E16" t="s">
         <v>28</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1015,7 +1015,7 @@
         <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E17" t="s">
         <v>28</v>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1032,7 +1032,7 @@
         <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E18" t="s">
         <v>31</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1049,7 +1049,7 @@
         <v>32</v>
       </c>
       <c r="D19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E19" t="s">
         <v>28</v>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1066,7 +1066,7 @@
         <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E20" t="s">
         <v>35</v>
@@ -1074,7 +1074,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -1083,7 +1083,7 @@
         <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E21" t="s">
         <v>36</v>
@@ -1091,7 +1091,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -1100,7 +1100,7 @@
         <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E22" t="s">
         <v>38</v>
@@ -1108,7 +1108,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1117,7 +1117,7 @@
         <v>39</v>
       </c>
       <c r="D23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E23" t="s">
         <v>40</v>
@@ -1125,7 +1125,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1134,7 +1134,7 @@
         <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E24" t="s">
         <v>42</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1151,7 +1151,7 @@
         <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E25" t="s">
         <v>44</v>
@@ -1159,24 +1159,24 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
         <v>94</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>95</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>96</v>
-      </c>
-      <c r="E26" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -1185,7 +1185,7 @@
         <v>45</v>
       </c>
       <c r="D27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E27" t="s">
         <v>46</v>
@@ -1193,7 +1193,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1202,7 +1202,7 @@
         <v>47</v>
       </c>
       <c r="D28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E28" t="s">
         <v>48</v>

</xml_diff>